<commit_message>
updated parts lists (ASI labelling + 100mm lens)
</commit_message>
<xml_diff>
--- a/Parts-List/BeamExpansion-Parts.xlsx
+++ b/Parts-List/BeamExpansion-Parts.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshe\Documents\GitHub\LifeHackWebsite\Parts-List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\LifeHackWebsite\Parts-List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB216DA-0863-44DE-848E-A1AA5B57003C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CB1E71D6-4A5E-428E-852D-7E788AF99D93}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Beam Expansion Module" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="68">
   <si>
     <t>Supplier</t>
   </si>
@@ -231,17 +229,26 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Small Positive lens</t>
+  </si>
+  <si>
+    <t>f = 100 mm, Ø1" Achromatic Doublet, ARC: 400 - 700 nm </t>
+  </si>
+  <si>
+    <t>AC254-100-A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +284,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -307,7 +322,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -622,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CBCBE2-63C2-4DB1-896E-CE51649B3CDD}">
-  <dimension ref="A1:G55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,7 +814,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1036,7 +1051,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -1169,298 +1184,301 @@
         <v>43</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+    </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D32" s="4">
-        <v>122.55</v>
+        <v>5.95</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" ref="F32:F38" si="2">D32*E32</f>
-        <v>122.55</v>
+        <f t="shared" ref="F32:F37" si="2">D32*E32</f>
+        <v>5.95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D33" s="4">
-        <v>67.16</v>
+        <v>39.770000000000003</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" s="4">
         <f t="shared" si="2"/>
-        <v>67.16</v>
+        <v>39.770000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D34" s="4">
-        <v>5.95</v>
+        <v>9.18</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
         <f t="shared" si="2"/>
-        <v>5.95</v>
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D35" s="4">
-        <v>4.01</v>
+        <v>7.96</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4">
         <f t="shared" si="2"/>
-        <v>4.01</v>
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D36" s="4">
-        <v>9.18</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
+        <v>4.1900000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D37" s="4">
-        <v>7.96</v>
+        <v>22.73</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G37" t="s">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="4">
+        <v>3.86</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="6">
+        <f>D38*E38</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="4">
-        <v>22.73</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="4">
-        <f t="shared" si="2"/>
-        <v>22.73</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>49</v>
+      <c r="C39" t="s">
+        <v>67</v>
       </c>
       <c r="D39" s="4">
-        <v>3.86</v>
+        <v>60.87</v>
       </c>
       <c r="E39" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="6">
         <f>D39*E39</f>
-        <v>0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-      <c r="F40" s="4"/>
+        <v>60.87</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D42" s="4">
-        <v>81.97</v>
+        <v>122.55</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" ref="F42:F48" si="3">D42*E42</f>
-        <v>81.97</v>
+        <v>122.55</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D43" s="4">
-        <v>5.95</v>
+        <v>67.16</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" s="4">
         <f t="shared" si="3"/>
-        <v>5.95</v>
+        <v>67.16</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D44" s="4">
-        <v>4.01</v>
+        <v>5.95</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" s="4">
         <f t="shared" si="3"/>
-        <v>4.01</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D45" s="4">
-        <v>9.18</v>
+        <v>4.01</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G45" t="s">
-        <v>43</v>
+        <v>4.01</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D46" s="4">
-        <v>7.96</v>
+        <v>9.18</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1475,47 +1493,50 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D47" s="4">
-        <v>22.73</v>
+        <v>7.96</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="3"/>
-        <v>22.73</v>
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D48" s="4">
-        <v>117.41</v>
+        <v>22.73</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="3"/>
-        <v>117.41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
@@ -1529,55 +1550,242 @@
         <v>3.86</v>
       </c>
       <c r="E49" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="6">
         <f>D49*E49</f>
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="4">
+        <v>81.97</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" ref="F52:F58" si="4">D52*E52</f>
+        <v>81.97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="4">
+        <v>5.95</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="4"/>
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4.01</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="4"/>
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="4">
+        <v>9.18</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="4">
+        <v>7.96</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="4">
+        <v>22.73</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" si="4"/>
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="4">
+        <v>117.41</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" si="4"/>
+        <v>117.41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="4">
         <v>3.86</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
+      <c r="E59" s="5">
+        <v>1</v>
+      </c>
+      <c r="F59" s="6">
+        <f>D59*E59</f>
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D62" s="4">
         <v>79.569999999999993</v>
       </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="4">
-        <f>D52*E52</f>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4">
+        <f>D62*E62</f>
         <v>79.569999999999993</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="1"/>
-      <c r="D53" s="4"/>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+      <c r="D63" s="4"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F55" s="4">
-        <f>SUM(F3:F52)</f>
-        <v>1907.8800000000003</v>
+      <c r="F65" s="4">
+        <f>SUM(F3:F62)</f>
+        <v>2041.3900000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>